<commit_message>
Database collections spreadsheet updated - users collection added.
</commit_message>
<xml_diff>
--- a/_Project Documentation/Database collections - Baking Hot!.xlsx
+++ b/_Project Documentation/Database collections - Baking Hot!.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Recipe Types" sheetId="2" r:id="rId1"/>
     <sheet name="Recipes " sheetId="1" r:id="rId2"/>
+    <sheet name="Users" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>type</t>
   </si>
@@ -63,6 +64,24 @@
   </si>
   <si>
     <t>type_name</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>user_type</t>
+  </si>
+  <si>
+    <t>Collection: recipe_types</t>
+  </si>
+  <si>
+    <t>Collection: users</t>
   </si>
 </sst>
 </file>
@@ -415,7 +434,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -430,7 +449,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -465,7 +484,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -575,4 +594,66 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>